<commit_message>
update file, code, and text for the C14 modeling file
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/KWL_C14_dates.xlsx
+++ b/analysis/data/raw_data/KWL_C14_dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Papers/kwl-pottery-2019/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705C41F7-85AD-4644-8365-7B4A95993335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8F8B8A-EB34-0749-A1C5-9B4D9ED03913}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="460" windowWidth="22680" windowHeight="16540" xr2:uid="{8DD15795-9B77-D142-AB16-8DEEBD71ECC9}"/>
+    <workbookView xWindow="3060" yWindow="1540" windowWidth="22680" windowHeight="16540" xr2:uid="{8DD15795-9B77-D142-AB16-8DEEBD71ECC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="119">
   <si>
     <t>L7</t>
   </si>
@@ -379,6 +379,18 @@
   </si>
   <si>
     <t>burial M095</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>upper</t>
+  </si>
+  <si>
+    <t>sterile</t>
   </si>
 </sst>
 </file>
@@ -747,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44DE8E0-CB48-C741-8CBC-BBB68EC49E9D}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -761,6 +773,7 @@
     <col min="7" max="7" width="7.6640625" customWidth="1"/>
     <col min="8" max="8" width="9.5" customWidth="1"/>
     <col min="9" max="9" width="24.5" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -791,6 +804,9 @@
       <c r="I1" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -820,6 +836,9 @@
       <c r="I2" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -850,6 +869,9 @@
       <c r="I3" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -879,6 +901,9 @@
       <c r="I4" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -902,6 +927,9 @@
       <c r="I5" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="J5" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -925,6 +953,9 @@
       <c r="I6" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="J6" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -954,6 +985,9 @@
       <c r="I7" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="J7" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -977,6 +1011,9 @@
       <c r="I8" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="J8" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1006,6 +1043,9 @@
       <c r="I9" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="J9" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1035,6 +1075,9 @@
       <c r="I10" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="J10" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1058,6 +1101,9 @@
       <c r="I11" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="J11" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1087,6 +1133,9 @@
       <c r="I12" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="J12" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1110,6 +1159,9 @@
       <c r="I13" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="J13" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="14" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1139,6 +1191,9 @@
       <c r="I14" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="J14" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="15" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1162,6 +1217,9 @@
       <c r="I15" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="J15" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="16" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1191,8 +1249,11 @@
       <c r="I16" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="J16" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
@@ -1220,8 +1281,11 @@
       <c r="I17" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="J17" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
@@ -1249,8 +1313,11 @@
       <c r="I18" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="J18" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>53</v>
       </c>
@@ -1278,8 +1345,11 @@
       <c r="I19" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="J19" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -1307,8 +1377,11 @@
       <c r="I20" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="J20" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>59</v>
       </c>
@@ -1336,8 +1409,11 @@
       <c r="I21" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="J21" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>61</v>
       </c>
@@ -1365,8 +1441,11 @@
       <c r="I22" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="J22" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>64</v>
       </c>
@@ -1388,8 +1467,11 @@
       <c r="I23" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="J23" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
@@ -1411,8 +1493,11 @@
       <c r="I24" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="J24" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
@@ -1440,8 +1525,11 @@
       <c r="I25" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="J25" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>69</v>
       </c>
@@ -1469,8 +1557,11 @@
       <c r="I26" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="J26" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -1498,8 +1589,11 @@
       <c r="I27" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="J27" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>75</v>
       </c>
@@ -1527,8 +1621,11 @@
       <c r="I28" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="J28" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>78</v>
       </c>
@@ -1556,8 +1653,11 @@
       <c r="I29" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="J29" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>82</v>
       </c>
@@ -1585,8 +1685,11 @@
       <c r="I30" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="J30" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>84</v>
       </c>
@@ -1614,8 +1717,11 @@
       <c r="I31" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="J31" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>88</v>
       </c>
@@ -1642,6 +1748,9 @@
       </c>
       <c r="I32" s="1" t="s">
         <v>98</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>